<commit_message>
Ajout données ASDEP et pop départementales
</commit_message>
<xml_diff>
--- a/data-raw/Contenu fichiers excel.xlsx
+++ b/data-raw/Contenu fichiers excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="386">
   <si>
     <t xml:space="preserve">NoOngletExcel</t>
   </si>
@@ -629,394 +629,400 @@
     <t xml:space="preserve">TotBenefPA_TotDepBruteAideSoc</t>
   </si>
   <si>
+    <t xml:space="preserve">DepBruteAPAdom_DepBruteAPAetab_DepNetteASH_DepBruteAccueilPAparticuliers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA-tab3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'APA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NbBenefAPA_DepBruteTotPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAPAdom_DepBruteAPAetab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA-tab4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAidesPAdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'aides à domicile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotBenefPADomicile_DepBruteTotPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAPAdom_DepBruteAidesMenageresPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA-tab5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAPAdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NbBenefAPADomicile_DepBruteAidesPAdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA-tab6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAidesPAetab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'accueil en établissement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotBenefPAEtab_DepBruteTotPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAPAetab_DepNetteASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA-tab7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepNetteASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses nettes d'aide sociale à l'hébergement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA-tab8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAPAetab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'APA en établissement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NbBenefAPAEtab_DepBruteAPA_DepBruteAidesPAetab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH-tab1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepNetteAidesPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aides au personnes handicapées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses nettes d'aide sociale aux personnes handicapées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotBenefPH_TotDepNetteAideSoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH-tab2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAidesPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'aide sociale aux personnes handicapées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotBenefPH_TotDepBruteAideSoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAidesDomPH_DepBruteAidesAccueilPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH-tab3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAidesDomPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'aide aux PH à domicile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotBenefPHDomicile_DepBruteAidesPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH-tab4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteACTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'ACTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NbBenefACTP_DepBruteAidesPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH-tab5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBrutePCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes de PCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NbBenefPCH_DepBruteAidesPH_DepBruteAidesDomPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH-tab6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAidesAccueilPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aides à l'accueil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'aide à l'accueil des PH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotBenefPHEtab_DepBruteAidesPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH-tab7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAidesAccueiletabPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accueil en établissement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'accueil de PH en établissements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NbBenefAideHebergementPH_DepBruteAidesPH_DepBruteAidesAccueilPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASE-tab1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepNetteASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses nette!s d'ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotDepNetteAideSoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASE-tab2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotDepBruteAideSoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAllocASE_DepBruteAEDAEMO_DepBrutePrevSpe_DepBrutePlacementASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASE-tab3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAllocASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allocations d'ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'allocations d'ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASE-tab4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAEDAEMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actions éducatives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'AED ou AEMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotBenefAEDAEMO_DepBruteASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASE-tab5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBrutePrevSpe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prévention spécialisée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes de prévention spécialisée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASE-tab6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBrutePlacementASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes de placement à l'ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotEnfAccueillisASE_DepBruteASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBrutePlacementFamASE_DepBrutePlacementetabASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASE-tab7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBrutePlacementFamASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes de placement familial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotEnfASEPlacesFamillesAccueil_DepBruteASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASE-tab8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBrutePlacementetabASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placement en établissement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes de placement en établissement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotEnfASEPlacesEtab_DepBruteASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RSA-RMI tab1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepNetteInsertion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aides à l'insertion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses nettes d'insertion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RSA-RMI tab2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteInsertion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes d'insertion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteRSA_DepBruteInsertionRSA_DepBruteCUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RSA-RMI tab3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteRSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses de RSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NbAllocRSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RSA-RMI tab5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteInsertionRSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aides à l'insertion hors CUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses d'insertion hors CUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSA-RMI tab6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteCUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses de CUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">autres-tab1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepNetteAutreAideSoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Services communs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses de personnel et autres interventions sociales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteAutreAideSoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tot-tab1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total dépenses nettes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses nettes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepNetteTotPA_DepNetteAidesPH_DepNetteASE_DepNetteInsertion_DepNetteAutreAideSoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tot-tab2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total dépenses brutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dépenses brutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DepBruteTotPA_DepBruteAidesPH_DepBruteASE_DepBruteInsertion_DepBruteAutreAideSoc</t>
+  </si>
+  <si>
     <t xml:space="preserve">DepBruteAPAdom_DepBruteAPAetab_DepBruteASH_DepBruteAccueilPAparticuliers</t>
   </si>
   <si>
-    <t xml:space="preserve">PA-tab3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'APA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NbBenefAPA_DepBruteTotPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAPAdom_DepBruteAPAetab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA-tab4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAidesPAdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'aides à domicile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotBenefPADomicile_DepBruteTotPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAPAdom_DepBruteAidesMenageresPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA-tab5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAPAdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NbBenefAPADomicile_DepBruteAidesPAdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA-tab6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAidesPAetab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'accueil en établissement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotBenefPAEtab_DepBruteTotPA</t>
-  </si>
-  <si>
     <t xml:space="preserve">DepBruteAPAetab_DepBruteASH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA-tab7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepNetteASH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses nettes d'aide sociale à l'hébergement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA-tab8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAPAetab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'APA en établissement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NbBenefAPAEtab_DepBruteAPA_DepBruteAidesPAetab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH-tab1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepNetteAidesPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aides au personnes handicapées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses nettes d'aide sociale aux personnes handicapées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotBenefPH_TotDepNetteAideSoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH-tab2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAidesPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'aide sociale aux personnes handicapées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotBenefPH_TotDepBruteAideSoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAidesDomPH_DepBruteAidesAccueilPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH-tab3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAidesDomPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'aide aux PH à domicile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotBenefPHDomicile_DepBruteAidesPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH-tab4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteACTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'ACTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NbBenefACTP_DepBruteAidesPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH-tab5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBrutePCH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes de PCH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NbBenefPCH_DepBruteAidesPH_DepBruteAidesDomPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH-tab6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAidesAccueilPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aides à l'accueil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'aide à l'accueil des PH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotBenefPHEtab_DepBruteAidesPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH-tab7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAidesAccueiletabPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accueil en établissement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'accueil de PH en établissements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NbBenefAideHebergementPH_DepBruteAidesPH_DepBruteAidesAccueilPH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASE-tab1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepNetteASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses nette!s d'ASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotDepNetteAideSoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASE-tab2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'ASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotDepBruteAideSoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAllocASE_DepBruteAEDAEMO_DepBrutePrevSpe_DepBrutePlacementASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASE-tab3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAllocASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allocations d'ASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'allocations d'ASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASE-tab4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAEDAEMO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actions éducatives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'AED ou AEMO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotBenefAEDAEMO_DepBruteASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASE-tab5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBrutePrevSpe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prévention spécialisée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes de prévention spécialisée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASE-tab6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBrutePlacementASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Placements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes de placement à l'ASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotEnfAccueillisASE_DepBruteASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBrutePlacementFamASE_DepBrutePlacementetabASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASE-tab7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBrutePlacementFamASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes de placement familial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotEnfASEPlacesFamillesAccueil_DepBruteASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASE-tab8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBrutePlacementetabASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Placement en établissement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes de placement en établissement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotEnfASEPlacesEtab_DepBruteASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RSA-RMI tab1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepNetteInsertion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aides à l'insertion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses nettes d'insertion</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RSA-RMI tab2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteInsertion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes d'insertion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteRSA_DepBruteInsertionRSA_DepBruteCUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RSA-RMI tab3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteRSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses de RSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NbAllocRSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RSA-RMI tab5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteInsertionRSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aides à l'insertion hors CUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses d'insertion hors CUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSA-RMI tab6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteCUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses de CUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">autres-tab1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepNetteAutreAideSoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Services communs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses de personnel et autres interventions sociales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteAutreAideSoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tot-tab1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total dépenses nettes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses nettes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepNetteTotPA_DepNetteAidesPH_DepNetteASE_DepNetteInsertion_DepNetteAutreAideSoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tot-tab2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total dépenses brutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dépenses brutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DepBruteTotPA_DepBruteAidesPH_DepBruteASE_DepBruteInsertion_DepBruteAutreAideSoc</t>
   </si>
   <si>
     <t xml:space="preserve">DepBruteASH</t>
@@ -2774,8 +2780,8 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3466,7 +3472,7 @@
         <v>200</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>201</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3543,7 +3549,7 @@
         <v>218</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>219</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3568,21 +3574,21 @@
         <v>223</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>224</v>
@@ -4072,154 +4078,154 @@
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>309</v>
@@ -4228,57 +4234,57 @@
         <v>307</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>307</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>307</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>

</xml_diff>

<commit_message>
Maj données asdep 2019
</commit_message>
<xml_diff>
--- a/data-raw/Contenu fichiers excel.xlsx
+++ b/data-raw/Contenu fichiers excel.xlsx
@@ -5,14 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="SL_benef_2018" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="SL_benef_2017" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="SL_depenses_2018" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="SL_depenses_2017" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="MS" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="SL_benef_2019" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SL_benef_2018" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="SL_benef_2017" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="SL_depenses_2019" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="SL_depenses_2018" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="SL_depenses_2017" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="MS" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="386">
   <si>
     <t xml:space="preserve">NoOngletExcel</t>
   </si>
@@ -2034,6 +2036,752 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F43"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
@@ -2773,14 +3521,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3395,7 +4143,629 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="100.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>330</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4034,7 +5404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>

</xml_diff>

<commit_message>
Ajoute table ASDEPslbenefnat et corr fonction readSheetDrees
</commit_message>
<xml_diff>
--- a/data-raw/Contenu fichiers excel.xlsx
+++ b/data-raw/Contenu fichiers excel.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="SL_benef_2020" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="SL_benef_2019" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="SL_benef_2018" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="SL_benef_2017" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="SL_depenses_2020" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="SL_depenses_2019" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="SL_depenses_2018" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="SL_depenses_2017" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="MS" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="SL_benef_2022" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SL_benef_2020" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="SL_benef_2019" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="SL_benef_2018" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="SL_benef_2017" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="SL_depenses_2020" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="SL_depenses_2019" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="SL_depenses_2018" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="SL_depenses_2017" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="MS" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="396">
   <si>
     <t xml:space="preserve">NoOngletExcel</t>
   </si>
@@ -1322,8 +1323,8 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2099,7 +2100,273 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="1:1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -2112,16 +2379,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.37"/>
@@ -2526,6 +2793,9 @@
       <c r="D22" s="0" t="s">
         <v>103</v>
       </c>
+      <c r="E22" s="0" t="s">
+        <v>82</v>
+      </c>
       <c r="F22" s="0" t="s">
         <v>104</v>
       </c>
@@ -2543,6 +2813,9 @@
       <c r="D23" s="0" t="s">
         <v>108</v>
       </c>
+      <c r="E23" s="0" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -2557,6 +2830,9 @@
       <c r="D24" s="0" t="s">
         <v>112</v>
       </c>
+      <c r="E24" s="0" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
@@ -2571,281 +2847,318 @@
       <c r="D25" s="0" t="s">
         <v>116</v>
       </c>
+      <c r="E25" s="0" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>128</v>
+        <v>119</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>132</v>
+        <v>123</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>136</v>
+        <v>127</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>170</v>
+        <v>160</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>194</v>
+        <v>186</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B45" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C45" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D45" s="0" t="s">
         <v>198</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -2861,7 +3174,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3606,8 +3919,8 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4350,22 +4663,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="100.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.97"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4390,570 +4702,695 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>201</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>203</v>
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>204</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>205</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>201</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>206</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>207</v>
+        <v>7</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>208</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>209</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>210</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>211</v>
+        <v>19</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>212</v>
+        <v>7</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>213</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>214</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>215</v>
+        <v>22</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>216</v>
+        <v>24</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>217</v>
+        <v>25</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>218</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>219</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>220</v>
+        <v>28</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>211</v>
+        <v>30</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>221</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>222</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>223</v>
+        <v>33</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>224</v>
+        <v>35</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>226</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>227</v>
+        <v>37</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>228</v>
+        <v>38</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>229</v>
+        <v>40</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>53</v>
+        <v>25</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>230</v>
+        <v>42</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>231</v>
+        <v>43</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>232</v>
+        <v>45</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>233</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>234</v>
+        <v>47</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>235</v>
+        <v>48</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>236</v>
+        <v>49</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>237</v>
+        <v>50</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>238</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>239</v>
+        <v>52</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>240</v>
+        <v>53</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>236</v>
+        <v>54</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>241</v>
+        <v>55</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>242</v>
+        <v>17</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>243</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>244</v>
+        <v>57</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>245</v>
+        <v>58</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>246</v>
+        <v>60</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>247</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>248</v>
+        <v>61</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>249</v>
+        <v>62</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>250</v>
+        <v>64</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>251</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>252</v>
+        <v>65</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>253</v>
+        <v>66</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>115</v>
+        <v>67</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>254</v>
+        <v>68</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>255</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>256</v>
+        <v>69</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>257</v>
+        <v>70</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>258</v>
+        <v>71</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>259</v>
+        <v>72</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>260</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>261</v>
+        <v>73</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>262</v>
+        <v>74</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>263</v>
+        <v>75</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>264</v>
+        <v>76</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>265</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>266</v>
+        <v>77</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>267</v>
+        <v>78</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>268</v>
+        <v>79</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>269</v>
+        <v>80</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>270</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>271</v>
+        <v>81</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>272</v>
+        <v>82</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>268</v>
+        <v>83</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>274</v>
+        <v>84</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>275</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>276</v>
+        <v>86</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>277</v>
+        <v>87</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>278</v>
+        <v>88</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>279</v>
+        <v>14</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>272</v>
+        <v>82</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>280</v>
+        <v>90</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>281</v>
+        <v>91</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>282</v>
+        <v>92</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>283</v>
+        <v>93</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>284</v>
+        <v>82</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>285</v>
+        <v>95</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>286</v>
+        <v>96</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>287</v>
+        <v>97</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>288</v>
+        <v>98</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>272</v>
+        <v>82</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>289</v>
+        <v>100</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>290</v>
+        <v>101</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>291</v>
+        <v>102</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>293</v>
+        <v>103</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>294</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>295</v>
+        <v>105</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>296</v>
+        <v>106</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>169</v>
+        <v>107</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>298</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>299</v>
+        <v>109</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>300</v>
+        <v>110</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>301</v>
+        <v>111</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>303</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>304</v>
+        <v>113</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>305</v>
+        <v>114</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>306</v>
+        <v>115</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>270</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>308</v>
+        <v>124</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>309</v>
+        <v>125</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>306</v>
+        <v>126</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>274</v>
+        <v>127</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>311</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>312</v>
+        <v>129</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>313</v>
+        <v>130</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>314</v>
+        <v>131</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>316</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>317</v>
+        <v>133</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>318</v>
+        <v>134</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>319</v>
+        <v>135</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>316</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>321</v>
+        <v>137</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>322</v>
+        <v>138</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>316</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>325</v>
+        <v>141</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>326</v>
+        <v>142</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>327</v>
+        <v>143</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>270</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>329</v>
+        <v>145</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>330</v>
+        <v>146</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>327</v>
+        <v>147</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>274</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>331</v>
+        <v>149</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>270</v>
+        <v>150</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>332</v>
+        <v>151</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>334</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>335</v>
+        <v>153</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>274</v>
+        <v>154</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>336</v>
+        <v>155</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>338</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -4974,8 +5411,8 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5596,8 +6033,8 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6100,7 +6537,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>339</v>
+        <v>317</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>318</v>
@@ -6117,7 +6554,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>322</v>
@@ -6151,7 +6588,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>330</v>
@@ -6216,10 +6653,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6288,7 +6725,7 @@
         <v>207</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>341</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6365,7 +6802,7 @@
         <v>225</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>342</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6390,348 +6827,348 @@
         <v>230</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>343</v>
+        <v>231</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>344</v>
+        <v>232</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>345</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>346</v>
+        <v>234</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>34</v>
+        <v>236</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>236</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>236</v>
+        <v>13</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>115</v>
+        <v>258</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>268</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>272</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>272</v>
+        <v>293</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>291</v>
+        <v>169</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>169</v>
+        <v>301</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>303</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>306</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>312</v>
+        <v>339</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>316</v>
@@ -6739,16 +7176,16 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>316</v>
@@ -6756,19 +7193,19 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>316</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6776,7 +7213,7 @@
         <v>325</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>327</v>
@@ -6785,57 +7222,40 @@
         <v>328</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>330</v>
+        <v>270</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>274</v>
+        <v>333</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="F34" s="0" t="s">
         <v>338</v>
       </c>
     </row>
@@ -6855,21 +7275,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="100.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.36"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6892,218 +7313,590 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="B11" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>316</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>386</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>338</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>